<commit_message>
Characters & schemas OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="334">
   <si>
     <t>Family</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>ref : acceptStatement, uponEnvironmentName</t>
-  </si>
-  <si>
-    <t>// Names for runtime structures</t>
   </si>
   <si>
     <t>alphabetName</t>
@@ -900,9 +897,6 @@
 If you choose a mnemonic-name that is also an environment-name, its definition as a mnemonic-name will take precedence over its definition as an environment-name.</t>
   </si>
   <si>
-    <t>// Data Conditions</t>
-  </si>
-  <si>
     <t>conditionForUPSISwitchName</t>
   </si>
   <si>
@@ -986,6 +980,165 @@
   </si>
   <si>
     <t>dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReference</t>
+  </si>
+  <si>
+    <t>Characters &amp; schemas</t>
+  </si>
+  <si>
+    <t>// Characters &amp; schemas</t>
+  </si>
+  <si>
+    <t>// Data &amp; Conditions</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>SymbolicCharacter</t>
+  </si>
+  <si>
+    <t>symbolicCharactersOrdinalPositions</t>
+  </si>
+  <si>
+    <t>symbolicCharacterDefinition</t>
+  </si>
+  <si>
+    <t>The same symbolic-character can appear only once in a SYMBOLIC CHARACTERS clause.</t>
+  </si>
+  <si>
+    <t>symbolic-character-1 is a user-defined word and must contain at least one alphabetic character.  
+The symbolic character can be a DBCS user-defined word.</t>
+  </si>
+  <si>
+    <t>symbolicCharacterReference</t>
+  </si>
+  <si>
+    <t>figurativeConstant</t>
+  </si>
+  <si>
+    <t>&gt;&gt;alphanumericLiteral
+&gt;&gt;alphanumericOrNationalLiteral</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You can use a figurative constant wherever literal appears in a syntax diagram, except where explicitly prohibited.</t>
+  </si>
+  <si>
+    <t>AlphabetName</t>
+  </si>
+  <si>
+    <t>alphabetClause</t>
+  </si>
+  <si>
+    <t>xml schema</t>
+  </si>
+  <si>
+    <t>character code set
+collating sequence</t>
+  </si>
+  <si>
+    <t>alphabetNameDefinition</t>
+  </si>
+  <si>
+    <t>symbolicCharactersClause</t>
+  </si>
+  <si>
+    <t>codeSetClause</t>
+  </si>
+  <si>
+    <t>mergeStatement</t>
+  </si>
+  <si>
+    <t>programCollatingSequenceClause</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alphabet-name-1 specifies a collating sequence when used in:
+- The PROGRAM COLLATING SEQUENCE clause of the object-computer paragraph
+- The COLLATING SEQUENCE phrase of the SORT or MERGE statement 
+alphabet-name-1 specifies a character code set when used in:
+- The FD entry CODE-SET clause
+- The SYMBOLIC CHARACTERS clause</t>
+  </si>
+  <si>
+    <t>objectComputerParagraph</t>
+  </si>
+  <si>
+    <t>alphabetNameReference</t>
+  </si>
+  <si>
+    <t>The collating sequence used in this program is the collating sequence associated with the specified alphabet-name.
+The collating sequence pertains to this program and to any programs that this program might contain.</t>
+  </si>
+  <si>
+    <t>fileDescriptionEntry</t>
+  </si>
+  <si>
+    <t>If the IN phrase is specified, integer-1 specifies the ordinal position of the character that is represented in the character set named by alphabet-name-2. This ordinal position must exist.</t>
+  </si>
+  <si>
+    <t>When the CODE-SET clause is specified, an alphabet-name identifies the character code convention used to represent data on the input-output device.
+alphabet-name must be defined in the SPECIAL-NAMES paragraph as STANDARD-1 (for ASCII-encoded files), STANDARD-2 (for ISO 7-bit encoded files), EBCDIC (for EBCDIC-encoded files), or NATIVE.</t>
+  </si>
+  <si>
+    <t>This phrase specifies the collating sequence to be used in alphanumeric comparisons for the KEY data items in this merge operation.
+alphabet-name-1 Must be specified in the ALPHABET clause of the SPECIAL-NAMES paragraph. 
+Any one of the alphabet-name clause phrases can be specified</t>
+  </si>
+  <si>
+    <t>This phrase specifies the collating sequence to be used in alphanumeric comparisons for the KEY data items in this sorting operation.
+alphabet-name-1 Must be specified in the ALPHABET clause of the SPECIAL-NAMES paragraph. 
+Any one of the alphabet-name clause phrases can be specified</t>
+  </si>
+  <si>
+    <t>classClause</t>
+  </si>
+  <si>
+    <t>set of characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The class-name in the CLASS clause can be a DBCS user-defined word. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">class-name-1 can be referenced only in a class condition. </t>
+  </si>
+  <si>
+    <t>&gt;&gt;conditionalExpression</t>
+  </si>
+  <si>
+    <t>classCondition</t>
+  </si>
+  <si>
+    <t>The class condition determines whether the content of a data item is in the set of characters specified by the CLASS clause as defined in the SPECIAL-NAMES paragraph of the ENVIRONMENT DIVISION.</t>
+  </si>
+  <si>
+    <t>characterClassNameReference</t>
+  </si>
+  <si>
+    <t>characterClassNameDefinition</t>
+  </si>
+  <si>
+    <t>xmlSchemaClause</t>
+  </si>
+  <si>
+    <t>XmlSchemaName</t>
+  </si>
+  <si>
+    <t>CharacterClassName</t>
+  </si>
+  <si>
+    <t>The xml-schema-name in the XML SCHEMA clause can be a DBCS user-defined word.</t>
+  </si>
+  <si>
+    <t>xmlSchemaNameDefinition</t>
+  </si>
+  <si>
+    <t>xml-schema-name-1 can be referenced only in an XML PARSE statement.</t>
+  </si>
+  <si>
+    <t>xmlSchemaNameReference</t>
+  </si>
+  <si>
+    <t>xml-schema-name-1 identifies an existing z/OS UNIX file or MVS data set that contains the optimized XML schema.
+xml-schema-name-1 must be associated with the external file name of the schema by using the XML-SCHEMA clause.</t>
   </si>
 </sst>
 </file>
@@ -1426,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C173"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,12 +1668,12 @@
     <row r="21" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1541,7 +1694,7 @@
     <row r="28" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1587,537 +1740,537 @@
     </row>
     <row r="40" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="52" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="54" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="56" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="58" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="60" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="14" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
-        <v>179</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>185</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>89</v>
+      <c r="B101" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>90</v>
+      <c r="C103" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>91</v>
+      <c r="C104" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>92</v>
+      <c r="C105" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C108" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
-        <v>96</v>
+      <c r="A109" t="s">
+        <v>97</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="B110" t="s">
         <v>98</v>
       </c>
-      <c r="B112" s="9" t="s">
-        <v>172</v>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
+      <c r="A113" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>101</v>
       </c>
     </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>102</v>
+      <c r="B118" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="B120" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>104</v>
+      <c r="A121" t="s">
+        <v>105</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>105</v>
+      <c r="B122" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>104</v>
+      <c r="A123" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>106</v>
-      </c>
-      <c r="B124" s="9" t="s">
+      <c r="B124" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
-        <v>109</v>
+      <c r="B126" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>110</v>
-      </c>
-      <c r="B128" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="14" t="s">
-        <v>116</v>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="11" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="11" t="s">
-        <v>178</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>173</v>
+      <c r="A141" s="11" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="11" t="s">
-        <v>180</v>
+      <c r="A142" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="10" t="s">
-        <v>123</v>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="159" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="160" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B160" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="164" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="165" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="166" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="167" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B167" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="168" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="169" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B169" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="170" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="171" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B171" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="172" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="173" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B173" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2128,14 +2281,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7605" ySplit="600" topLeftCell="A7" activePane="bottomRight"/>
-      <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:C11"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A10" activePane="bottomLeft"/>
+      <selection sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,13 +2321,13 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2188,10 +2339,10 @@
         <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>20</v>
@@ -2211,28 +2362,28 @@
         <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2240,34 +2391,34 @@
         <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K3" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2281,25 +2432,25 @@
         <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2313,28 +2464,28 @@
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2342,7 +2493,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2351,19 +2502,19 @@
         <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="225" x14ac:dyDescent="0.25">
@@ -2371,28 +2522,28 @@
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2406,124 +2557,249 @@
         <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K9" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K10" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="H11" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>269</v>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2534,14 +2810,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5175" ySplit="600" topLeftCell="A20" activePane="bottomRight"/>
-      <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A29" activePane="bottomLeft"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,22 +2839,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -2592,7 +2866,7 @@
         <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2602,26 +2876,26 @@
         <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2632,23 +2906,23 @@
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="105" x14ac:dyDescent="0.25">
@@ -2656,26 +2930,26 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2686,22 +2960,22 @@
         <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2709,25 +2983,25 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2735,25 +3009,25 @@
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2761,25 +3035,25 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2787,25 +3061,25 @@
         <v>15</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2813,25 +3087,25 @@
         <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="120" x14ac:dyDescent="0.25">
@@ -2839,25 +3113,25 @@
         <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2868,22 +3142,22 @@
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>220</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2894,19 +3168,19 @@
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2917,22 +3191,22 @@
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -2943,22 +3217,22 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2969,22 +3243,22 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2992,25 +3266,25 @@
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>228</v>
-      </c>
       <c r="I17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3021,19 +3295,19 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -3044,240 +3318,456 @@
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I20" s="4"/>
       <c r="K20" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F22" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="G26" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="H26" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SymbolInformation correctly attached to CodeElement instead of Token Data names OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="374">
   <si>
     <t>Family</t>
   </si>
@@ -1144,12 +1144,6 @@
     <t>ConditionName</t>
   </si>
   <si>
-    <t>condition : UPSI switch status</t>
-  </si>
-  <si>
-    <t>condition : data value</t>
-  </si>
-  <si>
     <t>dataConditionEntry</t>
   </si>
   <si>
@@ -1172,6 +1166,109 @@
   </si>
   <si>
     <t>qualifiedConditionName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>data item</t>
+  </si>
+  <si>
+    <t>condition on UPSI switch status</t>
+  </si>
+  <si>
+    <t>condition on data item value</t>
+  </si>
+  <si>
+    <t>DataName</t>
+  </si>
+  <si>
+    <t>dataNameDefinition</t>
+  </si>
+  <si>
+    <t>"
+dataRenamesEntry</t>
+  </si>
+  <si>
+    <t>data-name-1, if specified, identifies a data item used in the program.</t>
+  </si>
+  <si>
+    <t>redefinesClause</t>
+  </si>
+  <si>
+    <t>renamesClause</t>
+  </si>
+  <si>
+    <t>paddingCharacterClause</t>
+  </si>
+  <si>
+    <t>recordKeyClause</t>
+  </si>
+  <si>
+    <t>alternateRecordKeyClause</t>
+  </si>
+  <si>
+    <t>relativeKeyClause</t>
+  </si>
+  <si>
+    <t>passwordClause</t>
+  </si>
+  <si>
+    <t>fileStatusClause</t>
+  </si>
+  <si>
+    <t>fileControlEntry</t>
+  </si>
+  <si>
+    <t>recordClause</t>
+  </si>
+  <si>
+    <t>labelRecordsClause</t>
+  </si>
+  <si>
+    <t>valueOfClause</t>
+  </si>
+  <si>
+    <t>dataRecordsClause</t>
+  </si>
+  <si>
+    <t>linageClause</t>
+  </si>
+  <si>
+    <t>inputParameters</t>
+  </si>
+  <si>
+    <t>procedureDivisionHeader</t>
+  </si>
+  <si>
+    <t>returningPhrase</t>
+  </si>
+  <si>
+    <t>occursDependingOn</t>
+  </si>
+  <si>
+    <t>occursKeys</t>
+  </si>
+  <si>
+    <t>qualifiedDataName</t>
+  </si>
+  <si>
+    <t>dataNameReference</t>
+  </si>
+  <si>
+    <t>dataNameReference
+dataNameReferenceOrFileNameReference</t>
+  </si>
+  <si>
+    <t>&gt;&gt;identifier
+&gt;&gt;conditionalExpression
+readStatement
+releaseStatement
+rewriteStatement
+whenSearchCondition
+sortStatement
+startStatement
+writeStatement</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1295,6 +1392,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1612,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B70"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,33 +1975,33 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="73" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="14" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2309,12 +2412,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A9" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A10" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,7 +2778,7 @@
         <v>251</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>261</v>
@@ -2798,36 +2901,33 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>322</v>
+        <v>231</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>349</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2835,7 +2935,7 @@
         <v>332</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>334</v>
@@ -2844,19 +2944,56 @@
         <v>231</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G22" s="4" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2867,12 +3004,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A33" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G36:G37"/>
+      <pane ySplit="600" topLeftCell="A46" activePane="bottomLeft"/>
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,52 +3937,47 @@
         <v>319</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B35" s="4"/>
+        <v>332</v>
+      </c>
       <c r="C35" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>197</v>
+        <v>347</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>359</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>56</v>
+        <v>353</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>328</v>
+        <v>371</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>341</v>
+        <v>347</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>359</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>60</v>
+        <v>354</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>340</v>
+        <v>371</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>142</v>
@@ -3855,40 +3987,502 @@
       <c r="A37" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D55" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="F55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G55" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G56" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C39"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C40"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C41"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C42"/>
+      <c r="H56" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+    </row>
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="17"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="18"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C61" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Index name and File name OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -16,6 +16,9 @@
     <sheet name="Definitions" sheetId="1" r:id="rId2"/>
     <sheet name="References" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">References!$G$1:$G$78</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="406">
   <si>
     <t>Family</t>
   </si>
@@ -572,9 +575,6 @@
     <t xml:space="preserve"> programEntryDefinition</t>
   </si>
   <si>
-    <t>=fileName with IsRecord=true</t>
-  </si>
-  <si>
     <t>functionName // values : ACOS, ANNUITY, ASIN, ATAN, CHAR, COS, CURRENT-DATE, DATE-OF-INTEGER, DATE-TO-YYYYMMDD, DAY-OF-INTEGER, DAY-TO-YYYYDDD, DISPLAY-OF, FACTORIAL, INTEGER, INTEGER-OF-DATE, INTEGER-OF-DAY, INTEGER-PART, LENGTH, LOG, LOG10, LOWER-CASE, MAX, MEAN, MEDIAN, MIDRANGE, MIN, MOD, NATIONAL-OF, NUMVAL, NUMVAL-C, ORD, ORD-MAX, ORD-MIN, PRESENT-VALUE, RANDOM, RANGE, REM, REVERSE, SIN, SQRT, STANDARD-DEVIATION, SUM, TAN, ULENGTH, UPOS, UPPER-CASE, USUBSTR, USUPPLEMENTARY, UVALID, UWIDTH, VARIANCE, WHEN-COMPILED, YEAR-TO-YYYY</t>
   </si>
   <si>
@@ -1260,8 +1260,82 @@
 dataNameReferenceOrFileNameReference</t>
   </si>
   <si>
-    <t>&gt;&gt;identifier
-&gt;&gt;conditionalExpression
+    <t>=dataName with IsRecord=true</t>
+  </si>
+  <si>
+    <t>table index</t>
+  </si>
+  <si>
+    <t>IndexName</t>
+  </si>
+  <si>
+    <t>occursClause</t>
+  </si>
+  <si>
+    <t>indexNameDefinition</t>
+  </si>
+  <si>
+    <t>Unreferenced index names need not be uniquely defined.</t>
+  </si>
+  <si>
+    <t>If a data item that possesses the global attribute includes a table accessed with an index, that index also possesses the global attribute. 
+Therefore, the scope of an index-name is the same as that of the data-name that names the table in which the index is defined.
+Indexes specified in an external data record do not possess the external attribute.</t>
+  </si>
+  <si>
+    <t>These index-names are not data-names and are not identified elsewhere in the COBOL program; 
+instead, they can be regarded as private special registers that the compiler generates for working with a table for the use of this object program only.
+They are not data and are not part of any data hierarchy.
+In one table entry, up to 12 index-names can be specified.</t>
+  </si>
+  <si>
+    <t>"
+performVarying</t>
+  </si>
+  <si>
+    <t>searchStatement</t>
+  </si>
+  <si>
+    <t>setStatementForIndexes</t>
+  </si>
+  <si>
+    <t>indexNameReference</t>
+  </si>
+  <si>
+    <t>operand</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>selectClause</t>
+  </si>
+  <si>
+    <t>fileNameDefinition</t>
+  </si>
+  <si>
+    <t>A file-name must conform to the rules for a COBOL user-defined name, must contain at least one alphabetic character</t>
+  </si>
+  <si>
+    <t>file-name must be unique within this program.</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>identifierOrIndexName</t>
+  </si>
+  <si>
+    <t>qualifiedDataNameOrIndexName</t>
+  </si>
+  <si>
+    <t>dataNameReferenceOrIndexNameReference</t>
+  </si>
+  <si>
+    <t>&gt;&gt;conditionalExpression
 readStatement
 releaseStatement
 rewriteStatement
@@ -1269,6 +1343,66 @@
 sortStatement
 startStatement
 writeStatement</t>
+  </si>
+  <si>
+    <t>dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrIndexNameReference</t>
+  </si>
+  <si>
+    <t>&gt;&gt;conditionalExpression
+performProcedureStatement
+searchStatement</t>
+  </si>
+  <si>
+    <t>"
+"
+operand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+dataNameReferenceOrFileNameReference</t>
+  </si>
+  <si>
+    <t>fileNameReference</t>
+  </si>
+  <si>
+    <t>callBy</t>
+  </si>
+  <si>
+    <t>identifierOrFileName</t>
+  </si>
+  <si>
+    <t>&gt;&gt;identifier
+ioControlEntry
+fileDescriptionEntry
+useStatement
+closeStatement
+deleteStatement
+mergeStatement
+openStatement
+readStatement
+returnStatement
+sortStatement
+startStatement</t>
+  </si>
+  <si>
+    <t>linageCounterSpecialRegisterDecl
+rerunClause
+sameAreaClause
+multipleFileTapeClause
+applyWriteOnlyClause
+"
+useStatementForExceptionDeclarative
+closeFileName
+"
+"
+openIO/openExtend/fileNameWithNoRewindOrReversed/fileNameWithNoRewind
+"
+"
+"/usingFilenames/givingFilenames
+"</t>
+  </si>
+  <si>
+    <t>dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrFileNameReference</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1398,6 +1532,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1715,8 +1855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD73"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99:C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,12 +1944,12 @@
     <row r="21" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1830,7 +1970,7 @@
     <row r="28" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1876,7 +2016,7 @@
     </row>
     <row r="40" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1886,28 +2026,28 @@
     </row>
     <row r="42" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1957,7 +2097,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2005,93 +2145,93 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="74" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+    <row r="75" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
+    <row r="76" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
+    <row r="77" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="78" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+    <row r="79" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
+    <row r="80" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+    <row r="81" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="83" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+    <row r="84" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="86" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+    <row r="90" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+    <row r="91" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
+    <row r="92" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="14" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2100,43 +2240,43 @@
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+    <row r="98" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="99" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
+    <row r="100" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
+    <row r="101" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
+    <row r="102" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
+    <row r="103" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
+    <row r="104" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="14" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2145,7 +2285,7 @@
         <v>96</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>170</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2193,7 +2333,7 @@
         <v>104</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2216,7 +2356,7 @@
         <v>108</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,37 +2391,37 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2321,17 +2461,17 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2412,12 +2552,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A10" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,16 +2712,16 @@
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2604,19 +2744,19 @@
         <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2624,7 +2764,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2639,13 +2779,13 @@
         <v>3</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="225" x14ac:dyDescent="0.25">
@@ -2653,28 +2793,28 @@
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>136</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2697,30 +2837,30 @@
         <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>140</v>
@@ -2729,30 +2869,30 @@
         <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K9" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>141</v>
@@ -2761,30 +2901,30 @@
         <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K10" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>141</v>
@@ -2793,207 +2933,274 @@
         <v>60</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>289</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>296</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>297</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K14" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>334</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>335</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>337</v>
+    </row>
+    <row r="17" spans="1:13" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>333</v>
+        <v>385</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>323</v>
+        <v>386</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>246</v>
+        <v>358</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="D19" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G19" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G22" s="4" t="s">
-        <v>343</v>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G23" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -3004,12 +3211,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A46" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <pane ySplit="600" topLeftCell="A73" activePane="bottomLeft"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,7 +3225,7 @@
     <col min="2" max="2" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="5" customWidth="1"/>
@@ -3033,7 +3240,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
@@ -3070,7 +3277,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>149</v>
@@ -3082,7 +3289,7 @@
         <v>155</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="5" t="s">
@@ -3109,7 +3316,7 @@
         <v>156</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
@@ -3124,7 +3331,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>148</v>
@@ -3136,7 +3343,7 @@
         <v>155</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
@@ -3163,7 +3370,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>142</v>
@@ -3177,25 +3384,25 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -3203,25 +3410,25 @@
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -3229,25 +3436,25 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -3255,25 +3462,25 @@
         <v>15</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -3281,25 +3488,25 @@
         <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="120" x14ac:dyDescent="0.25">
@@ -3307,25 +3514,25 @@
         <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3336,22 +3543,22 @@
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>218</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3362,7 +3569,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>136</v>
@@ -3371,7 +3578,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>142</v>
@@ -3385,22 +3592,22 @@
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -3411,22 +3618,22 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3437,7 +3644,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>136</v>
@@ -3446,13 +3653,13 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3460,25 +3667,25 @@
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>136</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3489,7 +3696,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>136</v>
@@ -3498,7 +3705,7 @@
         <v>21</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>142</v>
@@ -3512,27 +3719,27 @@
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>142</v>
@@ -3541,13 +3748,13 @@
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>140</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>136</v>
@@ -3557,28 +3764,28 @@
       </c>
       <c r="I20" s="4"/>
       <c r="K20" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>141</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>136</v>
@@ -3588,74 +3795,74 @@
       </c>
       <c r="I21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F22" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>272</v>
-      </c>
       <c r="H23" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>136</v>
@@ -3664,18 +3871,18 @@
         <v>42</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -3685,322 +3892,324 @@
         <v>148</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="G26" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H26" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="H27" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K31" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="H31" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>302</v>
+        <v>245</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>136</v>
+        <v>299</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="K32" s="6" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K32" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>196</v>
+        <v>307</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>136</v>
+        <v>300</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B34" s="4"/>
+        <v>329</v>
+      </c>
+      <c r="B34" s="6"/>
       <c r="C34" s="4" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K36" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>142</v>
@@ -4008,22 +4217,22 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>142</v>
@@ -4031,22 +4240,22 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>142</v>
@@ -4054,22 +4263,22 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>142</v>
@@ -4077,22 +4286,22 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>308</v>
+        <v>346</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>358</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>142</v>
@@ -4100,22 +4309,22 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>308</v>
+        <v>346</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>358</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>142</v>
@@ -4123,22 +4332,22 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>142</v>
@@ -4146,22 +4355,22 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>142</v>
@@ -4169,22 +4378,22 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>142</v>
@@ -4192,22 +4401,22 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>142</v>
@@ -4215,22 +4424,22 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>142</v>
@@ -4238,253 +4447,666 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>366</v>
+        <v>230</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>366</v>
+        <v>230</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>373</v>
+        <v>346</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>365</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F52" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>372</v>
+      <c r="G52" s="4" t="s">
+        <v>370</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D53" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K55" s="13"/>
+    </row>
+    <row r="56" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="F53" s="16" t="s">
+      <c r="F56" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="G56" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G57" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="H53" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="H57" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I57" s="20"/>
+    </row>
+    <row r="58" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B58" s="20"/>
+      <c r="C58" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H58" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="H61" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I61" s="20"/>
+    </row>
+    <row r="62" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H62" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I62" s="20"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I64" s="20"/>
+    </row>
+    <row r="65" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I65" s="20"/>
+    </row>
+    <row r="66" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I66" s="20"/>
+    </row>
+    <row r="67" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H67" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I67" s="20"/>
+    </row>
+    <row r="68" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I68" s="20"/>
+    </row>
+    <row r="69" spans="1:11" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="F69" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I69" s="20"/>
+    </row>
+    <row r="70" spans="1:11" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I70" s="20"/>
+    </row>
+    <row r="71" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F73" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="G73" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K73" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="H58" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C59" s="17"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C60" s="18"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C61" s="18"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C74" s="17"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C75" s="18"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C76" s="18"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="13"/>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" s="13"/>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" s="13"/>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G89" s="6"/>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G93"/>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G78"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
External names and Special registers OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Notes" sheetId="3" r:id="rId1"/>
-    <sheet name="Definitions" sheetId="1" r:id="rId2"/>
-    <sheet name="References" sheetId="2" r:id="rId3"/>
+    <sheet name="Definitions" sheetId="1" r:id="rId1"/>
+    <sheet name="References" sheetId="2" r:id="rId2"/>
+    <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">References!$G$1:$G$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">References!$G$1:$G$79</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="430">
   <si>
     <t>Family</t>
   </si>
@@ -1404,12 +1404,115 @@
   <si>
     <t>dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrFileNameReference</t>
   </si>
+  <si>
+    <t>TextName</t>
+  </si>
+  <si>
+    <t>LibraryName</t>
+  </si>
+  <si>
+    <t>AssignmentName</t>
+  </si>
+  <si>
+    <t>copyCompilerStatement</t>
+  </si>
+  <si>
+    <t>copyCompilerStatementBody</t>
+  </si>
+  <si>
+    <t>libraryName</t>
+  </si>
+  <si>
+    <t>basisCompilerStatement</t>
+  </si>
+  <si>
+    <t>basisName</t>
+  </si>
+  <si>
+    <t>Neither text-name nor library-name need to be unique within a program.
+They can be identical to other user-defined words in the program.
+The uniqueness of text-name and library-name is determined after the formation and conversion rules for a system-dependent name have been applied.</t>
+  </si>
+  <si>
+    <t>text-name identifies the copy text.
+- Can be from 1-30 characters in length
+- Can contain the following characters: Latin uppercase letters A-Z, Latin lowercase letters a-z, digits 0-9, and hyphen
+- The first or last character must not be a hyphen
+- Cannot contain an underscore
+- Literals can contain characters: A-Z, a-z, 0-9, hyphen, @, #, or $.
+- For literals, only the first eight characters are used as the identifying name.</t>
+  </si>
+  <si>
+    <t>library-name identifies where the copy text exists.
+- Can be from 1-30 characters in length
+- Can contain the following characters: Latin uppercase letters A-Z, Latin lowercase letters a-z, digits 0-9, and hyphen
+- The first or last character must not be a hyphen
+- Cannot contain an underscore
+- Literals can contain characters: A-Z, a-z, 0-9, hyphen, @, #, or $.
+- For literals, only the first eight characters are used as the identifying name.
+text-name need not be qualified. If text-name is not qualified, a library-name of SYSLIB is assumed.</t>
+  </si>
+  <si>
+    <t>Same as textName</t>
+  </si>
+  <si>
+    <t>fileControlEntry
+fileControlEntry
+ioControlEntry</t>
+  </si>
+  <si>
+    <t>assignClause
+recordDelimiterClause
+rerunClause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assignment-name-1 Identifies the external data file. 
+It can be specified as a name or as an alphanumeric literal. 
+assignment-name-1 is not the name of a data item, and assignment-name-1 cannot be contained in a data item.
+ It is just a character string. It cannot contain an underscore character. </t>
+  </si>
+  <si>
+    <t>Specifies a user-defined word that must conform to the following rules:
+- The user-defined word can contain one to eight characters.
+- The user-defined word can contain the characters, A-Z, a-z, 0-9.
+- The leading character must be alphabetic.
+Specifies an alphanumeric literal that must conform to the following rules:
+- The literal can contain one to eight characters.
+- The literal can contain the characters, A-Z, a-z, 0-9, @, #, and $.
+- The leading character must be alphabetic, @, #, and $.</t>
+  </si>
+  <si>
+    <t>Runtime functions</t>
+  </si>
+  <si>
+    <t>FunctionName</t>
+  </si>
+  <si>
+    <t>execStatement</t>
+  </si>
+  <si>
+    <t>functionIdentifier</t>
+  </si>
+  <si>
+    <t>execTranslatorName</t>
+  </si>
+  <si>
+    <t>function-name-1 must be one of the intrinsic function names.</t>
+  </si>
+  <si>
+    <t>intrinsicFunctionName</t>
+  </si>
+  <si>
+    <t>&gt;&gt;identfier
+&gt;&gt;identifierOrIndexName
+&gt;&gt;identifierOrFileName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1440,13 +1543,6 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1513,22 +1609,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1538,6 +1630,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1853,709 +1949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C170"/>
-  <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99:C104"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C77" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C81" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C92" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C102" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C103" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C104" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>96</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>104</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>108</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A10" activePane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A16" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="bottomLeft" activeCell="G17" sqref="G17:G18"/>
     </sheetView>
@@ -3209,14 +2606,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A73" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A58" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,7 +2629,9 @@
     <col min="9" max="9" width="5.7109375" style="5" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" style="4" customWidth="1"/>
     <col min="11" max="11" width="131.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="4"/>
+    <col min="12" max="12" width="55.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="60" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3288,7 +2687,7 @@
       <c r="F2" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>187</v>
       </c>
       <c r="H2" s="8"/>
@@ -3315,7 +2714,7 @@
       <c r="F3" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>186</v>
       </c>
       <c r="H3" s="8"/>
@@ -3342,7 +2741,7 @@
       <c r="F4" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>188</v>
       </c>
       <c r="H4" s="8"/>
@@ -3369,7 +2768,7 @@
       <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>185</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -3626,7 +3025,7 @@
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>234</v>
       </c>
       <c r="H15" s="5" t="s">
@@ -3678,7 +3077,7 @@
       <c r="F17" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>225</v>
       </c>
       <c r="I17" s="5" t="s">
@@ -3704,7 +3103,7 @@
       <c r="F18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="14" t="s">
         <v>240</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -3921,7 +3320,7 @@
       <c r="E26" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="15" t="s">
         <v>280</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -3931,60 +3330,60 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="H27" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="28" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="H27" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:12" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H28" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I28" s="20"/>
+      <c r="H28" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12" t="s">
         <v>260</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -3993,7 +3392,7 @@
       <c r="E29" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="12" t="s">
         <v>402</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -4199,13 +3598,13 @@
       <c r="C37" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="16" t="s">
         <v>358</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F37" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -4222,13 +3621,13 @@
       <c r="C38" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="16" t="s">
         <v>358</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -4245,13 +3644,13 @@
       <c r="C39" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="16" t="s">
         <v>358</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F39" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -4268,13 +3667,13 @@
       <c r="C40" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="16" t="s">
         <v>358</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -4291,13 +3690,13 @@
       <c r="C41" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="16" t="s">
         <v>358</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F41" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -4314,13 +3713,13 @@
       <c r="C42" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="16" t="s">
         <v>358</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -4343,7 +3742,7 @@
       <c r="E43" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="F43" s="18" t="s">
+      <c r="F43" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -4366,7 +3765,7 @@
       <c r="E44" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -4389,7 +3788,7 @@
       <c r="E45" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F45" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -4412,7 +3811,7 @@
       <c r="E46" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -4435,7 +3834,7 @@
       <c r="E47" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="F47" s="18" t="s">
+      <c r="F47" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -4458,7 +3857,7 @@
       <c r="E48" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="F48" s="18" t="s">
+      <c r="F48" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -4468,7 +3867,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>331</v>
       </c>
@@ -4481,7 +3880,7 @@
       <c r="E49" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="F49" s="18" t="s">
+      <c r="F49" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -4491,7 +3890,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>331</v>
       </c>
@@ -4504,7 +3903,7 @@
       <c r="E50" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="F50" s="18" t="s">
+      <c r="F50" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -4514,7 +3913,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>331</v>
       </c>
@@ -4527,7 +3926,7 @@
       <c r="E51" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -4537,7 +3936,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>331</v>
       </c>
@@ -4550,7 +3949,7 @@
       <c r="E52" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="F52" s="18" t="s">
+      <c r="F52" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -4560,7 +3959,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>331</v>
       </c>
@@ -4573,7 +3972,7 @@
       <c r="E53" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="F53" s="18" t="s">
+      <c r="F53" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -4583,7 +3982,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>331</v>
       </c>
@@ -4596,7 +3995,7 @@
       <c r="E54" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F54" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G54" s="6" t="s">
@@ -4605,14 +4004,8 @@
       <c r="H54" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="L54" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="M54" s="4" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>331</v>
       </c>
@@ -4634,9 +4027,9 @@
       <c r="H55" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="K55" s="13"/>
-    </row>
-    <row r="56" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>331</v>
       </c>
@@ -4649,7 +4042,7 @@
       <c r="E56" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="G56" s="4" t="s">
@@ -4659,62 +4052,62 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+    <row r="57" spans="1:11" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="13" t="s">
+      <c r="B57" s="18"/>
+      <c r="C57" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="F57" s="13" t="s">
+      <c r="F57" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G57" s="13" t="s">
+      <c r="G57" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="H57" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I57" s="20"/>
-    </row>
-    <row r="58" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="H57" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58" spans="1:11" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="13" t="s">
+      <c r="B58" s="18"/>
+      <c r="C58" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F58" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G58" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H58" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I58" s="20"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="H58" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I58" s="18"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="13" t="s">
+      <c r="B59" s="18"/>
+      <c r="C59" s="12" t="s">
         <v>346</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -4723,7 +4116,7 @@
       <c r="E59" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F59" s="12" t="s">
         <v>402</v>
       </c>
       <c r="G59" s="4" t="s">
@@ -4733,380 +4126,1329 @@
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="B60" s="18"/>
+      <c r="C60" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E61" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F61" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G60" s="13" t="s">
+      <c r="G61" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="H60" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I60" s="20"/>
-    </row>
-    <row r="61" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="H61" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C62" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D62" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E62" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F62" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="G62" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="H61" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I61" s="20"/>
-    </row>
-    <row r="62" spans="1:13" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="H62" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63" spans="1:11" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C63" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D63" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E63" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F63" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="G62" s="13" t="s">
+      <c r="G63" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H62" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I62" s="20"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="H63" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D64" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F63" s="13" t="s">
+      <c r="F64" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="G64" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="H63" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="H64" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C65" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D65" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E65" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F65" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="G64" s="13" t="s">
+      <c r="G65" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H64" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I64" s="20"/>
-    </row>
-    <row r="65" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+      <c r="H65" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I65" s="18"/>
+    </row>
+    <row r="66" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C66" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D66" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="E65" s="13" t="s">
+      <c r="E66" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="F65" s="13" t="s">
+      <c r="F66" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="G65" s="13" t="s">
+      <c r="G66" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H65" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I65" s="20"/>
-    </row>
-    <row r="66" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+      <c r="H66" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C67" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D67" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="E67" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="F66" s="13" t="s">
+      <c r="F67" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G66" s="13" t="s">
+      <c r="G67" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="H66" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I66" s="20"/>
-    </row>
-    <row r="67" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
+      <c r="H67" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C68" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D68" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="E67" s="13" t="s">
+      <c r="E68" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F68" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="G67" s="13" t="s">
+      <c r="G68" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H67" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I67" s="20"/>
-    </row>
-    <row r="68" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+      <c r="H68" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C69" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="D68" s="13" t="s">
+      <c r="D69" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="E68" s="13" t="s">
+      <c r="E69" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="F68" s="13" t="s">
+      <c r="F69" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="G68" s="13" t="s">
+      <c r="G69" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="H68" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I68" s="20"/>
-    </row>
-    <row r="69" spans="1:11" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="H69" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C70" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D70" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="E70" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="F70" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="G70" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="H69" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I69" s="20"/>
-    </row>
-    <row r="70" spans="1:11" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+      <c r="H70" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71" spans="1:12" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C71" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D71" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="F70" s="18" t="s">
+      <c r="F71" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="G71" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="H70" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I70" s="20"/>
-    </row>
-    <row r="71" spans="1:11" ht="315" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="H71" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I71" s="18"/>
+    </row>
+    <row r="72" spans="1:12" ht="315" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13" t="s">
+      <c r="B72" s="12"/>
+      <c r="C72" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E72" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F72" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G71" s="4" t="s">
+      <c r="G72" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="H71" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="F72" s="13" t="s">
-        <v>402</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>405</v>
-      </c>
       <c r="H72" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>330</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="F74" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G73" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="H73" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K73" s="6" t="s">
+      <c r="H74" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K74" s="6" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C74" s="17"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C75" s="18"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C76" s="18"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83" s="13"/>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84" s="13"/>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85" s="13"/>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G89" s="6"/>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G92"/>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G93"/>
+    <row r="75" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G84" s="12"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G85" s="12"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G86" s="12"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G78"/>
+  <autoFilter ref="G1:G79"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C170"/>
+  <sheetViews>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>96</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B122" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct two remaining ambiguities : identifierOrClassName and assignmentNameOrFileNameReference
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">References!$G$1:$G$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">References!$G$1:$G$81</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="431">
   <si>
     <t>Family</t>
   </si>
@@ -741,9 +741,6 @@
     <t>#inheritsFromClassName</t>
   </si>
   <si>
-    <t>invokeObject</t>
-  </si>
-  <si>
     <t>usageClause</t>
   </si>
   <si>
@@ -803,9 +800,6 @@
     <t>See definition tab</t>
   </si>
   <si>
-    <t>classNameReferenceOrObjectReference</t>
-  </si>
-  <si>
     <t>When class-name-1 is specified together with literal-1 or identifier-2, the INVOKE statement invokes a static or factory method of the class referenced by class-name-1. 
 The method must be a static method if class-name-1 is a Java class; the method must be a factory method ifclass-name-1 is a COBOL class.
 When class-name-1 is specified together with NEW, the INVOKE statement creates a new object that is an instance of class class-name-1.
@@ -827,10 +821,6 @@
   </si>
   <si>
     <t>methodNameReference</t>
-  </si>
-  <si>
-    <t>methodNameReference
-methodNameFromData</t>
   </si>
   <si>
     <t>literal-1
@@ -1371,22 +1361,120 @@
     <t>identifierOrFileName</t>
   </si>
   <si>
-    <t>&gt;&gt;identifier
-ioControlEntry
-fileDescriptionEntry
-useStatement
-closeStatement
-deleteStatement
-mergeStatement
-openStatement
-readStatement
-returnStatement
-sortStatement
-startStatement</t>
+    <t>dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrFileNameReference</t>
+  </si>
+  <si>
+    <t>TextName</t>
+  </si>
+  <si>
+    <t>LibraryName</t>
+  </si>
+  <si>
+    <t>AssignmentName</t>
+  </si>
+  <si>
+    <t>copyCompilerStatement</t>
+  </si>
+  <si>
+    <t>copyCompilerStatementBody</t>
+  </si>
+  <si>
+    <t>libraryName</t>
+  </si>
+  <si>
+    <t>basisCompilerStatement</t>
+  </si>
+  <si>
+    <t>basisName</t>
+  </si>
+  <si>
+    <t>Neither text-name nor library-name need to be unique within a program.
+They can be identical to other user-defined words in the program.
+The uniqueness of text-name and library-name is determined after the formation and conversion rules for a system-dependent name have been applied.</t>
+  </si>
+  <si>
+    <t>text-name identifies the copy text.
+- Can be from 1-30 characters in length
+- Can contain the following characters: Latin uppercase letters A-Z, Latin lowercase letters a-z, digits 0-9, and hyphen
+- The first or last character must not be a hyphen
+- Cannot contain an underscore
+- Literals can contain characters: A-Z, a-z, 0-9, hyphen, @, #, or $.
+- For literals, only the first eight characters are used as the identifying name.</t>
+  </si>
+  <si>
+    <t>library-name identifies where the copy text exists.
+- Can be from 1-30 characters in length
+- Can contain the following characters: Latin uppercase letters A-Z, Latin lowercase letters a-z, digits 0-9, and hyphen
+- The first or last character must not be a hyphen
+- Cannot contain an underscore
+- Literals can contain characters: A-Z, a-z, 0-9, hyphen, @, #, or $.
+- For literals, only the first eight characters are used as the identifying name.
+text-name need not be qualified. If text-name is not qualified, a library-name of SYSLIB is assumed.</t>
+  </si>
+  <si>
+    <t>Same as textName</t>
+  </si>
+  <si>
+    <t>fileControlEntry
+fileControlEntry
+ioControlEntry</t>
+  </si>
+  <si>
+    <t>assignClause
+recordDelimiterClause
+rerunClause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assignment-name-1 Identifies the external data file. 
+It can be specified as a name or as an alphanumeric literal. 
+assignment-name-1 is not the name of a data item, and assignment-name-1 cannot be contained in a data item.
+ It is just a character string. It cannot contain an underscore character. </t>
+  </si>
+  <si>
+    <t>Specifies a user-defined word that must conform to the following rules:
+- The user-defined word can contain one to eight characters.
+- The user-defined word can contain the characters, A-Z, a-z, 0-9.
+- The leading character must be alphabetic.
+Specifies an alphanumeric literal that must conform to the following rules:
+- The literal can contain one to eight characters.
+- The literal can contain the characters, A-Z, a-z, 0-9, @, #, and $.
+- The leading character must be alphabetic, @, #, and $.</t>
+  </si>
+  <si>
+    <t>Runtime functions</t>
+  </si>
+  <si>
+    <t>FunctionName</t>
+  </si>
+  <si>
+    <t>execStatement</t>
+  </si>
+  <si>
+    <t>functionIdentifier</t>
+  </si>
+  <si>
+    <t>execTranslatorName</t>
+  </si>
+  <si>
+    <t>function-name-1 must be one of the intrinsic function names.</t>
+  </si>
+  <si>
+    <t>intrinsicFunctionName</t>
+  </si>
+  <si>
+    <t>identifierOrClassName</t>
+  </si>
+  <si>
+    <t>assignmentNameOrFileNameReference</t>
+  </si>
+  <si>
+    <t>rerunClause</t>
+  </si>
+  <si>
+    <t>ioControlEntry</t>
   </si>
   <si>
     <t>linageCounterSpecialRegisterDecl
-rerunClause
 sameAreaClause
 multipleFileTapeClause
 applyWriteOnlyClause
@@ -1402,110 +1490,24 @@
 "</t>
   </si>
   <si>
-    <t>dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrFileNameReference</t>
-  </si>
-  <si>
-    <t>TextName</t>
-  </si>
-  <si>
-    <t>LibraryName</t>
-  </si>
-  <si>
-    <t>AssignmentName</t>
-  </si>
-  <si>
-    <t>copyCompilerStatement</t>
-  </si>
-  <si>
-    <t>copyCompilerStatementBody</t>
-  </si>
-  <si>
-    <t>libraryName</t>
-  </si>
-  <si>
-    <t>basisCompilerStatement</t>
-  </si>
-  <si>
-    <t>basisName</t>
-  </si>
-  <si>
-    <t>Neither text-name nor library-name need to be unique within a program.
-They can be identical to other user-defined words in the program.
-The uniqueness of text-name and library-name is determined after the formation and conversion rules for a system-dependent name have been applied.</t>
-  </si>
-  <si>
-    <t>text-name identifies the copy text.
-- Can be from 1-30 characters in length
-- Can contain the following characters: Latin uppercase letters A-Z, Latin lowercase letters a-z, digits 0-9, and hyphen
-- The first or last character must not be a hyphen
-- Cannot contain an underscore
-- Literals can contain characters: A-Z, a-z, 0-9, hyphen, @, #, or $.
-- For literals, only the first eight characters are used as the identifying name.</t>
-  </si>
-  <si>
-    <t>library-name identifies where the copy text exists.
-- Can be from 1-30 characters in length
-- Can contain the following characters: Latin uppercase letters A-Z, Latin lowercase letters a-z, digits 0-9, and hyphen
-- The first or last character must not be a hyphen
-- Cannot contain an underscore
-- Literals can contain characters: A-Z, a-z, 0-9, hyphen, @, #, or $.
-- For literals, only the first eight characters are used as the identifying name.
-text-name need not be qualified. If text-name is not qualified, a library-name of SYSLIB is assumed.</t>
-  </si>
-  <si>
-    <t>Same as textName</t>
-  </si>
-  <si>
-    <t>fileControlEntry
-fileControlEntry
-ioControlEntry</t>
-  </si>
-  <si>
-    <t>assignClause
-recordDelimiterClause
-rerunClause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assignment-name-1 Identifies the external data file. 
-It can be specified as a name or as an alphanumeric literal. 
-assignment-name-1 is not the name of a data item, and assignment-name-1 cannot be contained in a data item.
- It is just a character string. It cannot contain an underscore character. </t>
-  </si>
-  <si>
-    <t>Specifies a user-defined word that must conform to the following rules:
-- The user-defined word can contain one to eight characters.
-- The user-defined word can contain the characters, A-Z, a-z, 0-9.
-- The leading character must be alphabetic.
-Specifies an alphanumeric literal that must conform to the following rules:
-- The literal can contain one to eight characters.
-- The literal can contain the characters, A-Z, a-z, 0-9, @, #, and $.
-- The leading character must be alphabetic, @, #, and $.</t>
-  </si>
-  <si>
-    <t>Runtime functions</t>
-  </si>
-  <si>
-    <t>FunctionName</t>
-  </si>
-  <si>
-    <t>execStatement</t>
-  </si>
-  <si>
-    <t>functionIdentifier</t>
-  </si>
-  <si>
-    <t>execTranslatorName</t>
-  </si>
-  <si>
-    <t>function-name-1 must be one of the intrinsic function names.</t>
-  </si>
-  <si>
-    <t>intrinsicFunctionName</t>
+    <t>&gt;&gt;identifier
+ioControlEntry
+fileDescriptionEntry
+useStatement
+closeStatement
+deleteStatement
+mergeStatement
+openStatement
+readStatement
+rerunStatement
+sortStatement
+startStatement</t>
   </si>
   <si>
     <t>&gt;&gt;identfier
 &gt;&gt;identifierOrIndexName
-&gt;&gt;identifierOrFileName</t>
+&gt;&gt;identifierOrFileName
+&gt;&gt;identifierOrClassName</t>
   </si>
 </sst>
 </file>
@@ -1952,9 +1954,9 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A4" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17:G18"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2163,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2176,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>142</v>
@@ -2190,28 +2192,28 @@
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>136</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2240,24 +2242,24 @@
         <v>142</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>140</v>
@@ -2266,30 +2268,30 @@
         <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>141</v>
@@ -2298,30 +2300,30 @@
         <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>141</v>
@@ -2330,274 +2332,274 @@
         <v>60</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>261</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="H12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>346</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>331</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>379</v>
-      </c>
       <c r="L17" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>88</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>56</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G23" s="4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -2608,12 +2610,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A58" activePane="bottomLeft"/>
+      <pane ySplit="600" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
@@ -2951,13 +2953,13 @@
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2977,7 +2979,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>142</v>
@@ -2991,22 +2993,22 @@
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -3017,22 +3019,22 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>218</v>
+        <v>136</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>234</v>
+        <v>424</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3043,7 +3045,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>136</v>
@@ -3052,13 +3054,13 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3066,25 +3068,25 @@
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>136</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3095,7 +3097,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>136</v>
@@ -3104,7 +3106,7 @@
         <v>21</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>142</v>
@@ -3118,27 +3120,27 @@
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E19" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>136</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>241</v>
-      </c>
       <c r="I19" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>142</v>
@@ -3147,13 +3149,13 @@
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>140</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>136</v>
@@ -3163,28 +3165,28 @@
       </c>
       <c r="I20" s="4"/>
       <c r="K20" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>141</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>136</v>
@@ -3194,74 +3196,74 @@
       </c>
       <c r="I21" s="4"/>
       <c r="K21" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>136</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>269</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>136</v>
@@ -3270,18 +3272,18 @@
         <v>42</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
@@ -3291,40 +3293,40 @@
         <v>148</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>281</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>142</v>
@@ -3332,22 +3334,22 @@
     </row>
     <row r="27" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>142</v>
@@ -3356,22 +3358,22 @@
     </row>
     <row r="28" spans="1:12" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H28" s="18" t="s">
         <v>142</v>
@@ -3380,23 +3382,23 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>149</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>142</v>
@@ -3404,122 +3406,122 @@
     </row>
     <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>136</v>
@@ -3528,22 +3530,22 @@
         <v>50</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>195</v>
@@ -3555,60 +3557,60 @@
         <v>50</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>53</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>142</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>142</v>
@@ -3616,22 +3618,22 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>142</v>
@@ -3639,22 +3641,22 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>142</v>
@@ -3662,22 +3664,22 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>142</v>
@@ -3685,22 +3687,22 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>142</v>
@@ -3708,22 +3710,22 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>142</v>
@@ -3731,22 +3733,22 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>142</v>
@@ -3754,22 +3756,22 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>142</v>
@@ -3777,22 +3779,22 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>142</v>
@@ -3800,22 +3802,22 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>142</v>
@@ -3823,22 +3825,22 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>142</v>
@@ -3846,22 +3848,22 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F48" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>142</v>
@@ -3869,22 +3871,22 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F49" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>142</v>
@@ -3892,22 +3894,22 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F50" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>142</v>
@@ -3915,22 +3917,22 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F51" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>142</v>
@@ -3938,22 +3940,22 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>142</v>
@@ -3961,22 +3963,22 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F53" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>142</v>
@@ -3984,22 +3986,22 @@
     </row>
     <row r="54" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>142</v>
@@ -4007,22 +4009,22 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>394</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>142</v>
@@ -4031,22 +4033,22 @@
     </row>
     <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F56" s="17" t="s">
         <v>67</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>142</v>
@@ -4054,23 +4056,23 @@
     </row>
     <row r="57" spans="1:11" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B57" s="18"/>
       <c r="C57" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>67</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H57" s="18" t="s">
         <v>142</v>
@@ -4079,23 +4081,23 @@
     </row>
     <row r="58" spans="1:11" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B58" s="18"/>
       <c r="C58" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H58" s="18" t="s">
         <v>142</v>
@@ -4104,38 +4106,38 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B59" s="18"/>
       <c r="C59" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>149</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B60" s="18"/>
       <c r="C60" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>136</v>
@@ -4152,22 +4154,22 @@
     </row>
     <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D61" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="E61" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>341</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H61" s="18" t="s">
         <v>142</v>
@@ -4176,22 +4178,22 @@
     </row>
     <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H62" s="18" t="s">
         <v>142</v>
@@ -4200,22 +4202,22 @@
     </row>
     <row r="63" spans="1:11" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H63" s="18" t="s">
         <v>142</v>
@@ -4224,23 +4226,23 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>149</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>142</v>
@@ -4248,22 +4250,22 @@
     </row>
     <row r="65" spans="1:12" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>199</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H65" s="18" t="s">
         <v>142</v>
@@ -4272,22 +4274,22 @@
     </row>
     <row r="66" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>136</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H66" s="18" t="s">
         <v>142</v>
@@ -4296,22 +4298,22 @@
     </row>
     <row r="67" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>148</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>83</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H67" s="18" t="s">
         <v>142</v>
@@ -4320,22 +4322,22 @@
     </row>
     <row r="68" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H68" s="18" t="s">
         <v>142</v>
@@ -4344,22 +4346,22 @@
     </row>
     <row r="69" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E69" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="G69" s="12" t="s">
         <v>391</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="G69" s="12" t="s">
-        <v>394</v>
       </c>
       <c r="H69" s="18" t="s">
         <v>142</v>
@@ -4368,22 +4370,22 @@
     </row>
     <row r="70" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F70" s="17" t="s">
         <v>88</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H70" s="18" t="s">
         <v>142</v>
@@ -4392,156 +4394,145 @@
     </row>
     <row r="71" spans="1:12" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F71" s="16" t="s">
         <v>88</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>142</v>
       </c>
       <c r="I71" s="18"/>
     </row>
-    <row r="72" spans="1:12" ht="315" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B72" s="12"/>
       <c r="C72" s="12" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>403</v>
+        <v>429</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>404</v>
+        <v>428</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>88</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>402</v>
+      <c r="A73" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
       <c r="D74" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G74" s="4" t="s">
+      <c r="G75" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="H74" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K74" s="6" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="F75" s="4" t="s">
+      <c r="B76" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K75" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="L75" s="6" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>413</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>101</v>
@@ -4552,95 +4543,98 @@
       <c r="I76" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="K76" s="4" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="K76" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C77" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="E77" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="L78" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K77" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="L77" s="6" t="s">
+    </row>
+    <row r="79" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="F78" s="4" t="s">
+      <c r="F79" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>106</v>
@@ -4652,103 +4646,165 @@
         <v>142</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K80" s="6"/>
+    </row>
+    <row r="81" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K81" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F82" s="20" t="s">
+        <v>423</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K82" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C81" s="4" t="s">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="E81" s="4" t="s">
+      <c r="D83" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F81" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G84" s="12"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G85" s="12"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F83" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G86" s="12"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G87" s="12"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C92" s="13"/>
       <c r="D92" s="13"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
     </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+    </row>
   </sheetData>
-  <autoFilter ref="G1:G79"/>
+  <autoFilter ref="G1:G81"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -4847,12 +4903,12 @@
     <row r="21" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4873,7 +4929,7 @@
     <row r="28" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4919,7 +4975,7 @@
     </row>
     <row r="40" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4929,13 +4985,13 @@
     </row>
     <row r="42" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5000,7 +5056,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5188,7 +5244,7 @@
         <v>96</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Study of CodeElements scope
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="References" sheetId="2" r:id="rId2"/>
-    <sheet name="Notes" sheetId="3" r:id="rId3"/>
+    <sheet name="Scope" sheetId="4" r:id="rId3"/>
+    <sheet name="Notes" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">References!$G$1:$G$81</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="537">
   <si>
     <t>Family</t>
   </si>
@@ -1509,12 +1510,377 @@
 &gt;&gt;identifierOrFileName
 &gt;&gt;identifierOrClassName</t>
   </si>
+  <si>
+    <t>User-defined words</t>
+  </si>
+  <si>
+    <t>udw single byte</t>
+  </si>
+  <si>
+    <t>Library name</t>
+  </si>
+  <si>
+    <t>Object-oriented class name</t>
+  </si>
+  <si>
+    <t>Program name</t>
+  </si>
+  <si>
+    <t>Text name</t>
+  </si>
+  <si>
+    <t>udw DBCS allowed</t>
+  </si>
+  <si>
+    <t>Alphabet name</t>
+  </si>
+  <si>
+    <t>Class name (of data)</t>
+  </si>
+  <si>
+    <t>Condition name</t>
+  </si>
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Index name</t>
+  </si>
+  <si>
+    <t>Mnemonic name</t>
+  </si>
+  <si>
+    <t>Paragraph name</t>
+  </si>
+  <si>
+    <t>Record name</t>
+  </si>
+  <si>
+    <t>Section name</t>
+  </si>
+  <si>
+    <t>Symbolic character</t>
+  </si>
+  <si>
+    <t>XML-schema name</t>
+  </si>
+  <si>
+    <t>System name</t>
+  </si>
+  <si>
+    <t>sn single byte</t>
+  </si>
+  <si>
+    <t>Language name</t>
+  </si>
+  <si>
+    <t>Implementor name</t>
+  </si>
+  <si>
+    <t>Environment name</t>
+  </si>
+  <si>
+    <t>External class name</t>
+  </si>
+  <si>
+    <t>External fileid</t>
+  </si>
+  <si>
+    <t>Assignment name</t>
+  </si>
+  <si>
+    <t>sn DBCS allowed</t>
+  </si>
+  <si>
+    <t>Computer name</t>
+  </si>
+  <si>
+    <t>// Symbols defined and referenced in the program</t>
+  </si>
+  <si>
+    <t>// External names referenced in the program</t>
+  </si>
+  <si>
+    <t>/// &lt;summary&gt;</t>
+  </si>
+  <si>
+    <t>/// Type to use when the parser can't determine the exact SymbolType.</t>
+  </si>
+  <si>
+    <t>/// The actual type will be resolved in a next compiler phase</t>
+  </si>
+  <si>
+    <t>/// &lt;/summary&gt;</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>MnemonicForEnvironmentName
+MnemonicForUPSISwitchName</t>
+  </si>
+  <si>
+    <t>(=DataName + IsRecord)</t>
+  </si>
+  <si>
+    <t>MethodName (Literal)</t>
+  </si>
+  <si>
+    <t>SpecialRegisterName (Keyword)</t>
+  </si>
+  <si>
+    <t>EnvironmentName
+UPSISwitchName</t>
+  </si>
+  <si>
+    <t>(= AssignmentName)</t>
+  </si>
+  <si>
+    <t>// p9: In COBOL words (but not in the content of alphanumeric, DBCS, and national</t>
+  </si>
+  <si>
+    <t>// literals), each lowercase single-byte alphabetic letter is considered to be equivalent</t>
+  </si>
+  <si>
+    <t>// to its corresponding single-byte uppercase alphabetic letter.</t>
+  </si>
+  <si>
+    <t>// p9: The following rules apply for all COBOL words:</t>
+  </si>
+  <si>
+    <t>// - A reserved word cannot be used as a user-defined word or as a system-name.</t>
+  </si>
+  <si>
+    <t>// - The same COBOL word, however, can be used as both a user-defined word and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//   as a system-name. </t>
+  </si>
+  <si>
+    <t>// p11: A given user-defined word can belong to only one of these sets, except that a given</t>
+  </si>
+  <si>
+    <t>// number can be both a priority-number and a level-number. Each user-defined</t>
+  </si>
+  <si>
+    <t>// word within a set must be unique, except for priority-numbers and level-numbers</t>
+  </si>
+  <si>
+    <t>// and except as specified in Chapter 8, “Referencing data names, copy libraries, and</t>
+  </si>
+  <si>
+    <t>// PROCEDURE DIVISION names,” on page 65.</t>
+  </si>
+  <si>
+    <t>Program + Contained pgms</t>
+  </si>
+  <si>
+    <t>// p12: A function-name specifies the mechanism provided to determine the value of an</t>
+  </si>
+  <si>
+    <t>// intrinsic function.</t>
+  </si>
+  <si>
+    <t>// The same word, in a different context, can appear in a program as a user-defined</t>
+  </si>
+  <si>
+    <t>// word or a system-name. For a list of function-names and their definitions, see</t>
+  </si>
+  <si>
+    <t>// Table 51 on page 485.</t>
+  </si>
+  <si>
+    <t>p79 =&gt; Chapter 7. Scope of names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data resource </t>
+  </si>
+  <si>
+    <t>COBOL programming element</t>
+  </si>
+  <si>
+    <t>record</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>global/local</t>
+  </si>
+  <si>
+    <t>local : Program
+global : Program + Contained pgms</t>
+  </si>
+  <si>
+    <t>SCOPE in programs</t>
+  </si>
+  <si>
+    <t>global ?</t>
+  </si>
+  <si>
+    <t>GLOBAL clause in entry or father entry</t>
+  </si>
+  <si>
+    <t>GLOBAL clause in file description entry</t>
+  </si>
+  <si>
+    <t>GLOBAL clause in record description entry or GLOBAL clause in father file description entry</t>
+  </si>
+  <si>
+    <t>always global</t>
+  </si>
+  <si>
+    <t>GLOBAL clause in father entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A separately compiled program and all of its directly and indirectly contained programs must have unique program-names within that separately compiled program.
+Names of programs that constitute a run unit are not necessarily unique, but when two programs in a run unit are identically named, at least one of the programs must be directly or indirectly contained </t>
+  </si>
+  <si>
+    <t>Any program of the run unit</t>
+  </si>
+  <si>
+    <t>SEPARATELY COMPILED programs
+Any program of the run unit
+Except contained programs
+NESTED programs
+local : Containing program
+global : Containing program + Contained programs - Except this program and its children</t>
+  </si>
+  <si>
+    <t>Is program nested ?
+Program with COMMON attribute ?</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Run unit =&gt; List of SEPARATELY COMPILED program names
+Program =&gt; List of directly EMBEDDED program names
+Walk up the embedded programs, program names are only visible from levels &lt;= current level if COMMON attribute and program not on path</t>
+  </si>
+  <si>
+    <t>always local</t>
+  </si>
+  <si>
+    <t>assigns a name in the PROCEDURE DIVISION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neither text-name nor library-name need to be unique within a program. They can be identical to other user-defined words in the program. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> identical to the scope of the data-name that includes the table</t>
+  </si>
+  <si>
+    <t>If a data item that possesses the global attribute includes a table accessed with an index, that index also possesses the global attribute</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>external ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A global name can be used to refer to the resource with which it is associated both: v From within the program in which the global name is declared v From within any other program that is contained in the program that declares the global name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A data item or file connector is external if the storage associated with that resource is associated with the run unit rather than with any particular program or method within the run unit. An external resource can be referenced by any program or method in the run unit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKING-STORAGE SECTION : presence of the EXTERNAL clause in the data description entry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data name
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file connector</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>EXTERNAL clause in entry or in father data descrpition entry or in father file description entry</t>
+  </si>
+  <si>
+    <t>EXTERNAL clause in file description entry
+Does not imply that the associated file-name is a global name</t>
+  </si>
+  <si>
+    <t>SEPARATELY COMPILED programs
+Any program of the run unit
+Except contained programs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the name is not declared in program B, the referenced resource is: 
+– The resource in program A if the name is declared in program A 
+– The resource in the containing program if the name is declared in the program that contains program A 
+This rule is applied to further containing programs until a valid resource is found</t>
+  </si>
+  <si>
+    <t>Within a class definition, resources can be defined within the following units: v The factory data division v The object data division v A method data division</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>In any hierarchy, the data-name associated with the highest level must be unique if it is referenced, and cannot be qualified.
+When programs are directly or indirectly contained within other programs, each program can use identical user-defined words to name resources
+You must specify enough qualification to make the name unique; however, it is not always necessary to specify all the levels of the hierarchy
+When programs are directly or indirectly contained within other programs, each program can use identical user-defined words to name resources</t>
+  </si>
+  <si>
+    <t>If library-name-1 is not specified, SYSLIB is assumed as the library name.</t>
+  </si>
+  <si>
+    <t>A section-name is the highest and only qualifier available for a paragraph-name and must be unique if referenced. PROCEDURE DIVISION names that are explicitly referenced in a program must be unique within a section.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program
+A paragraph-name or section-name that appears in a program cannot be referenced from any other program. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A section-name is the highest and only qualifier available for a paragraph-name and must be unique if referenced. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DATA DIVISION names that are explicitly referenced must either be uniquely defined or made unique through qualification. Unreferenced data items need not be uniquely defined. 
+identifier refers to a valid combination of a data-name or function-identifier with its qualifiers, subscripts, and reference-modifiers as required for uniqueness of reference.
+Each qualifier must be of a higher level than the name it qualifies and must be within the same hierarchy. </t>
+  </si>
+  <si>
+    <t>If explicitly referenced, a condition-name must be unique or be made unique through qualification or subscripting (or both) except when the scope of names by itself ensures uniqueness of reference.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,8 +1922,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1567,6 +1970,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,7 +1992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1636,6 +2045,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2612,10 +3053,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A7" activePane="bottomLeft"/>
       <selection activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,7 +3749,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>247</v>
       </c>
@@ -3332,7 +3773,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>247</v>
       </c>
@@ -4031,7 +4472,7 @@
       </c>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>328</v>
       </c>
@@ -4054,7 +4495,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>328</v>
       </c>
@@ -4368,7 +4809,7 @@
       </c>
       <c r="I69" s="18"/>
     </row>
-    <row r="70" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>327</v>
       </c>
@@ -4811,6 +5252,691 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="26.42578125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" style="26" customWidth="1"/>
+    <col min="10" max="10" width="43.28515625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="44.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+    </row>
+    <row r="2" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="F2" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>498</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>499</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>529</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>509</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>494</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>495</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>513</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>402</v>
+      </c>
+      <c r="P5" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>434</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>528</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E7" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>435</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>507</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>508</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31" t="s">
+        <v>505</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>510</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="P8" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>531</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>513</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>401</v>
+      </c>
+      <c r="P9" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>437</v>
+      </c>
+      <c r="P10" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>438</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="P11" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>439</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="P12" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>440</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>440</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>504</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>536</v>
+      </c>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="24" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+      <c r="C15" s="34" t="s">
+        <v>522</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>500</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" t="s">
+        <v>523</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>501</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="22" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>442</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>514</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>515</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="K17" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>443</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>444</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>511</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>534</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>532</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="22"/>
+    </row>
+    <row r="20" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="C20" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>502</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="22" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>446</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>511</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>447</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>448</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>449</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>453</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>454</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q29" s="23"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>455</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="K30" s="23" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>456</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>458</v>
+      </c>
+      <c r="L33" s="23" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L34" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q36" s="23"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>476</v>
+      </c>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="Q41" s="32" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>485</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>486</v>
+      </c>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>487</v>
+      </c>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>488</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>489</v>
+      </c>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C170"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update from @prudholu : added scope of names for our grammar study
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/Symbols and User defined words.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\TypeCobol\TypeCobol\Documentation\Studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMEDILOL\workspaces\TypeCobol\TypeCobol\Documentation\Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="References" sheetId="2" r:id="rId2"/>
-    <sheet name="Notes" sheetId="3" r:id="rId3"/>
+    <sheet name="Scope of name" sheetId="4" r:id="rId3"/>
+    <sheet name="Notes" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">References!$G$1:$G$81</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="541">
   <si>
     <t>Family</t>
   </si>
@@ -1509,12 +1510,518 @@
 &gt;&gt;identifierOrFileName
 &gt;&gt;identifierOrClassName</t>
   </si>
+  <si>
+    <t>ProgramEntry</t>
+  </si>
+  <si>
+    <t>IntrinsicFunctionName</t>
+  </si>
+  <si>
+    <t>DataTypeName</t>
+  </si>
+  <si>
+    <t>REFERENCE : structure of a Cobol compilation unit</t>
+  </si>
+  <si>
+    <t>ClassIdentification</t>
+  </si>
+  <si>
+    <t>EnvironmentDivisionHeader</t>
+  </si>
+  <si>
+    <t>configurationSection?</t>
+  </si>
+  <si>
+    <t>(FactoryIdentification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(DataDivisionHeader </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> workingStorageSection?</t>
+  </si>
+  <si>
+    <t>)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ProcedureDivisionHeader </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> methodDefinition*</t>
+  </si>
+  <si>
+    <t>FactoryEnd)?</t>
+  </si>
+  <si>
+    <t>(ObjectIdentification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">)?             </t>
+  </si>
+  <si>
+    <t>ObjectEnd)?</t>
+  </si>
+  <si>
+    <t>ClassEnd?;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">methodDefinition: </t>
+  </si>
+  <si>
+    <t>MethodIdentification</t>
+  </si>
+  <si>
+    <t>(EnvironmentDivisionHeader</t>
+  </si>
+  <si>
+    <t>inputOutputSection?</t>
+  </si>
+  <si>
+    <t>fileSection?</t>
+  </si>
+  <si>
+    <t>workingStorageSection?</t>
+  </si>
+  <si>
+    <t>localStorageSection?</t>
+  </si>
+  <si>
+    <t>linkageSection?</t>
+  </si>
+  <si>
+    <t>declaratives?</t>
+  </si>
+  <si>
+    <t>section*</t>
+  </si>
+  <si>
+    <t>MethodEnd;</t>
+  </si>
+  <si>
+    <t>cobolProgram:</t>
+  </si>
+  <si>
+    <t>ProgramIdentification</t>
+  </si>
+  <si>
+    <t>environmentDivision?</t>
+  </si>
+  <si>
+    <t>dataDivision?</t>
+  </si>
+  <si>
+    <t>procedureDivision?</t>
+  </si>
+  <si>
+    <t>nestedProgram=cobolProgram*</t>
+  </si>
+  <si>
+    <t>ProgramEnd?;</t>
+  </si>
+  <si>
+    <t>&lt;== only in outermost program</t>
+  </si>
+  <si>
+    <t>Defined in</t>
+  </si>
+  <si>
+    <t>Referenced in</t>
+  </si>
+  <si>
+    <t>Visibility</t>
+  </si>
+  <si>
+    <t>dataDescriptionEntry
+functionDataParameter</t>
+  </si>
+  <si>
+    <t>Defining scopes</t>
+  </si>
+  <si>
+    <t>Referencing scopes</t>
+  </si>
+  <si>
+    <t>SpecialNamesParagraph</t>
+  </si>
+  <si>
+    <t>Defining CodeElements</t>
+  </si>
+  <si>
+    <t>Program (not nested)
+Class</t>
+  </si>
+  <si>
+    <t>codeSetClause
+collatingSequence
+programCollatingSequenceClause
+symbolicCharactersClause</t>
+  </si>
+  <si>
+    <t>FileDescriptionEntry
+MergeStatement
+SortStatement
+ObjectComputerParagraph
+SpecialNamesParagraph</t>
+  </si>
+  <si>
+    <t>Referencing  code elements</t>
+  </si>
+  <si>
+    <t>Target Object</t>
+  </si>
+  <si>
+    <t>CollatingSequence</t>
+  </si>
+  <si>
+    <t>classIdentification
+repositoryClassDeclaration (def or ref)</t>
+  </si>
+  <si>
+    <t>ClassIdentification
+RepositoryParagraph</t>
+  </si>
+  <si>
+    <t>Program
+Class</t>
+  </si>
+  <si>
+    <t>See p123 : Identifying and referencing a class</t>
+  </si>
+  <si>
+    <t>repositoryClassDeclaration (def or ref)</t>
+  </si>
+  <si>
+    <t>RepositoryParagraph</t>
+  </si>
+  <si>
+    <t>ClassNode
+ExternalClassDescription</t>
+  </si>
+  <si>
+    <t>UserDefinedCollatingSequence</t>
+  </si>
+  <si>
+    <t>EvaluateStatement
+IfStatement
+PerformStatement
+SearchStatement</t>
+  </si>
+  <si>
+    <t>dataConditionEntry
+functionConditionParameter</t>
+  </si>
+  <si>
+    <t>classIdentification (inherits from)
+classEnd
+usageClause (object reference)
+repositoryClassDeclaration (def or ref)
+[[dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrClassNameReference]]=&gt;classNameOrObjectReferenceVariable</t>
+  </si>
+  <si>
+    <t>ClassIdentification
+ClassEnd
+DataDescriptionEntry / ParametersDescriptionEntry / FunctionCallResultDescriptionEntry 
+RepositoryParagraph
+InvokeStatement</t>
+  </si>
+  <si>
+    <t>Program
+Function
+Class
+Factory
+Object
+Method</t>
+  </si>
+  <si>
+    <t>Program
+Function
+Class
+Method</t>
+  </si>
+  <si>
+    <t>[[conditionNameReferenceOrConditionForUPSISwitchNameReference]]=&gt;conditionNameConditionOrSwitchStatusCondition=&gt;conditionalExpression/setStatementForConditions
+[[dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReference
+...OrIndexNameReference
+...OrFileNameReference
+...OrClassNameReference]]=&gt;identifier/indentifierOrFileName/identifierOrIndexName/identifierOrClassName</t>
+  </si>
+  <si>
+    <t>DataConditionEntry
+ParameterDescriptionEntry</t>
+  </si>
+  <si>
+    <t>Tuple&lt;ExternalName, UPSISwitchStatus&gt;</t>
+  </si>
+  <si>
+    <t>idem above ConditionName</t>
+  </si>
+  <si>
+    <t>dataDescriptionEntry
+dataRenamesEntry
+functionDataParameter</t>
+  </si>
+  <si>
+    <t>DataDescriptionEntry
+ParameterDescriptionEntry</t>
+  </si>
+  <si>
+    <t>Tuple&lt;StorageAreaNode,ConditionValueNode&gt;</t>
+  </si>
+  <si>
+    <t>StorageAreaNode</t>
+  </si>
+  <si>
+    <t>dataNameReference
+intrinsicDataNameReference
+...OrFileNameReference
+...OrIndexNameReference
+...OrFileNameReferenceOrMnemonicForUPSISwitchNameReference
+...OrConditionNameReferenceOrConditionForUPSISwitchNameReference
+..OrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrIndexNameReference
+...OrFileNameReference
+...OrClassNameReference</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">qualifiedDataName
+otherStorageAreaReference
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.. Many variables and sotrage areas ...</t>
+    </r>
+  </si>
+  <si>
+    <t>DataTypeDescriptionEntry</t>
+  </si>
+  <si>
+    <t>DataTypeNode</t>
+  </si>
+  <si>
+    <t>DataDescriptionEntry
+(+ Special Register + FunctionCallResult)
+DataRedefinesEntry
+DataRenamesEntry
+ParameterDescriptionEntry</t>
+  </si>
+  <si>
+    <t>DataDescriptionEntry
+(+ Special Register + FunctionCallResult)
+ParameterDescriptionEntry</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EvaluateStatement
+IfStatement
+PerformStatement
+SearchStatement
+SetStatement (for conditions)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Many statements or expressions</t>
+    </r>
+  </si>
+  <si>
+    <t>IndexRegister ?</t>
+  </si>
+  <si>
+    <t>indexStorageArea
+dataNameReferenceOrIndexNameReference=&gt;integerVariableOrIndex2=&gt;subscript=&gt;identifier
+dataNameReferenceOrConditionNameReferenceOrConditionForUPSISwitchNameReferenceOrIndexNameReference=&gt;identifierOrIndexName</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SetStatement (for indexes)
+SetStatement (for table handling)
+PerformStatement (loop variable)
+SearchStatement (serial varying)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.. Many variables and storage areas (subscript) …
+relationCondition
+signCondition</t>
+    </r>
+  </si>
+  <si>
+    <t>FileControlEntry</t>
+  </si>
+  <si>
+    <t>FileControlNode</t>
+  </si>
+  <si>
+    <t>Program
+Method</t>
+  </si>
+  <si>
+    <t>rerunClause
+sameAreaClause
+multipleFileTapeClause
+applyWriteOnlyClause
+fileDescriptionEntry
+useStatementForExceptionDeclarative
+closeFileDirective
+deleteStatement
+mergeStatement
+openStatement
+readStatement
+returnStatement
+sortStatement
+startStatement
+...OrFileNameReference=&gt;rerunClause/qualifiedDataName/qualifiedConditionName/sharedVariableOrFileName=&gt;CallStatement</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IoControlEntry
+FileDescriptionEntry
+CloseStatement
+DeleteStatement
+MergeStatement
+OpenStatement
+ReadStatement
+ReturnStatement
+SortStatement
+StartStatement
+UseAfterIOExceptionStatement
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.. Many variables and storage areas (subscript) …</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CallStatement (file parameter)</t>
+    </r>
+  </si>
+  <si>
+    <t>functionDeclarationHeader</t>
+  </si>
+  <si>
+    <t>FunctionDeclarationHeader</t>
+  </si>
+  <si>
+    <t>FunctionNode</t>
+  </si>
+  <si>
+    <t>userDefinedFunctionCall</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>any identifier</t>
+  </si>
+  <si>
+    <t>MethodNode</t>
+  </si>
+  <si>
+    <t>Factory
+Object</t>
+  </si>
+  <si>
+    <t>methodEnd
+invokeStatement</t>
+  </si>
+  <si>
+    <t>MethodEnd
+InvokeStatement</t>
+  </si>
+  <si>
+    <t>Program
+Function
+Method</t>
+  </si>
+  <si>
+    <t>acceptStatement
+displayStatement
+writeStatement</t>
+  </si>
+  <si>
+    <t>AcceptStatement
+DisplayStatement
+WriteStatement</t>
+  </si>
+  <si>
+    <t>SetStatement (for switches)</t>
+  </si>
+  <si>
+    <t>ExternalName</t>
+  </si>
+  <si>
+    <t>ParagraphHeader</t>
+  </si>
+  <si>
+    <t>PargraphNode</t>
+  </si>
+  <si>
+    <t>alterStatement
+gotoStatement
+mergeStatement
+performStatement
+sortStatement
+useStatement
+xmlParseStatement</t>
+  </si>
+  <si>
+    <t>alterStatement
+gotoStatement
+mergeStatement
+performStatement (procedure)
+sortStatement
+useStatement (for debugging)
+xmlParseStatement</t>
+  </si>
+  <si>
+    <t>Program (not nested)</t>
+  </si>
+  <si>
+    <t>EntryStatement</t>
+  </si>
+  <si>
+    <t>Tuple&lt;Program,EntryStatement&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,8 +2063,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1567,6 +2098,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,7 +2120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1636,6 +2173,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1953,13 +2511,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A4" activePane="bottomLeft"/>
-      <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -2612,13 +3169,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="5" bestFit="1" customWidth="1"/>
@@ -2884,7 +3440,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -2910,7 +3466,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -2985,7 +3541,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -3011,7 +3567,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -3112,7 +3668,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -3308,7 +3864,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>247</v>
       </c>
@@ -3332,7 +3888,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>247</v>
       </c>
@@ -4031,7 +4587,7 @@
       </c>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>328</v>
       </c>
@@ -4054,7 +4610,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>328</v>
       </c>
@@ -4368,7 +4924,7 @@
       </c>
       <c r="I69" s="18"/>
     </row>
-    <row r="70" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>327</v>
       </c>
@@ -4812,11 +5368,770 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I79"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="16" customWidth="1"/>
+    <col min="3" max="5" width="26.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="30" style="16" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>482</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>493</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>497</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>510</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>499</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>499</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>500</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>508</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>504</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>507</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>471</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>484</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>501</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>512</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="345" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>516</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>517</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>518</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>418</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>521</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>525</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>526</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>528</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>530</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>531</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>535</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>529</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>537</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>467</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="16" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="16" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="16" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="16" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="16" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="16" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="16" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="16" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="16" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="16" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="16" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>